<commit_message>
repo ready for class demo
</commit_message>
<xml_diff>
--- a/Code/Code/results.xlsx
+++ b/Code/Code/results.xlsx
@@ -136,6 +136,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Execution Time In</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Ticks vs. Input  Signal Length</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1032,11 +1062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1355063744"/>
-        <c:axId val="-1355055040"/>
+        <c:axId val="-1857328144"/>
+        <c:axId val="-1857326512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1355063744"/>
+        <c:axId val="-1857328144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,12 +1123,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1355055040"/>
+        <c:crossAx val="-1857326512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1355055040"/>
+        <c:axId val="-1857326512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1355063744"/>
+        <c:crossAx val="-1857328144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>